<commit_message>
fix: change some more final code a star
</commit_message>
<xml_diff>
--- a/Demo /A_star/Distance_Limit_Region.xlsx
+++ b/Demo /A_star/Distance_Limit_Region.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A414512E-0782-124F-8689-B1DBD6E01BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19B5B18-F168-0449-A614-AC7C3F82CEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>Dien Bien, Ha Giang &amp; Tuyen Quang</t>
-  </si>
-  <si>
-    <t>Cao Bang, Bac Kan &amp; Lang Son</t>
-  </si>
-  <si>
     <t>Central of Vietnam</t>
   </si>
   <si>
@@ -50,6 +44,48 @@
   </si>
   <si>
     <t>Distance Limit</t>
+  </si>
+  <si>
+    <t>21.3</t>
+  </si>
+  <si>
+    <t>22.9</t>
+  </si>
+  <si>
+    <t>103.1</t>
+  </si>
+  <si>
+    <t>21.6</t>
+  </si>
+  <si>
+    <t>22.7</t>
+  </si>
+  <si>
+    <t>105.83</t>
+  </si>
+  <si>
+    <t>106.76</t>
+  </si>
+  <si>
+    <t>105.3</t>
+  </si>
+  <si>
+    <t>15.8</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>19.9</t>
+  </si>
+  <si>
+    <t>15.13</t>
+  </si>
+  <si>
+    <t>Cao Bang &amp; Bac Kan &amp; Lang Son</t>
+  </si>
+  <si>
+    <t>Dien Bien &amp; Ha Giang &amp; Tuyen Quang</t>
   </si>
 </sst>
 </file>
@@ -65,18 +101,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA985"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -99,12 +129,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +424,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -406,41 +437,41 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>21.3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>22.9</v>
-      </c>
-      <c r="D2" s="1">
-        <v>103.1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>105.3</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <v>130</v>
@@ -448,19 +479,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>21.6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>22.7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>105.83</v>
-      </c>
-      <c r="E3" s="1">
-        <v>106.76</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="1">
         <v>120</v>
@@ -468,13 +499,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>19.899999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>103</v>
@@ -488,13 +519,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>10.9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>15.13</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>103</v>
@@ -508,7 +539,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>

</xml_diff>